<commit_message>
Fit deck matrix to hex values
</commit_message>
<xml_diff>
--- a/deck_matrix.xlsx
+++ b/deck_matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabrielu\Documents\GitHub\pythonUNO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabrielu\Documents\GitHub\pythonUNO\pythonUNO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{563F071A-BFA2-4D50-912A-5F85F574DBD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40021418-2143-478D-93C2-1746B9791935}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{B15789E7-B705-47E5-9885-1E92CB412029}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="11">
   <si>
     <t>B</t>
   </si>
@@ -56,12 +56,15 @@
   <si>
     <t>\</t>
   </si>
+  <si>
+    <t>F</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +75,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -173,6 +192,21 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -492,9 +526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{135F7D65-679A-4275-AD79-17A776C4C5ED}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -955,6 +991,611 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
     </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="11">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11">
+        <v>1</v>
+      </c>
+      <c r="D13" s="11">
+        <v>2</v>
+      </c>
+      <c r="E13" s="11">
+        <v>3</v>
+      </c>
+      <c r="F13" s="11">
+        <v>4</v>
+      </c>
+      <c r="G13" s="11">
+        <v>5</v>
+      </c>
+      <c r="H13" s="11">
+        <v>6</v>
+      </c>
+      <c r="I13" s="11">
+        <v>7</v>
+      </c>
+      <c r="J13" s="11">
+        <v>8</v>
+      </c>
+      <c r="K13" s="11">
+        <v>9</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q13" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="12">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1">
+        <v>3</v>
+      </c>
+      <c r="I14" s="1">
+        <v>4</v>
+      </c>
+      <c r="J14" s="1">
+        <v>5</v>
+      </c>
+      <c r="K14" s="1">
+        <v>6</v>
+      </c>
+      <c r="L14" s="1">
+        <v>7</v>
+      </c>
+      <c r="M14" s="1">
+        <v>8</v>
+      </c>
+      <c r="N14" s="1">
+        <v>9</v>
+      </c>
+      <c r="O14" s="1">
+        <v>1</v>
+      </c>
+      <c r="P14" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1">
+        <v>9</v>
+      </c>
+      <c r="H15" s="14">
+        <v>1</v>
+      </c>
+      <c r="I15" s="14">
+        <v>2</v>
+      </c>
+      <c r="J15" s="14">
+        <v>3</v>
+      </c>
+      <c r="K15" s="14">
+        <v>4</v>
+      </c>
+      <c r="L15" s="14">
+        <v>5</v>
+      </c>
+      <c r="M15" s="14">
+        <v>6</v>
+      </c>
+      <c r="N15" s="14">
+        <v>7</v>
+      </c>
+      <c r="O15" s="14">
+        <v>8</v>
+      </c>
+      <c r="P15" s="14">
+        <v>9</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12">
+        <v>2</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3">
+        <v>5</v>
+      </c>
+      <c r="F16" s="3">
+        <v>6</v>
+      </c>
+      <c r="G16" s="3">
+        <v>7</v>
+      </c>
+      <c r="H16" s="3">
+        <v>8</v>
+      </c>
+      <c r="I16" s="3">
+        <v>9</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>2</v>
+      </c>
+      <c r="L16" s="4">
+        <v>3</v>
+      </c>
+      <c r="M16" s="4">
+        <v>4</v>
+      </c>
+      <c r="N16" s="4">
+        <v>5</v>
+      </c>
+      <c r="O16" s="4">
+        <v>6</v>
+      </c>
+      <c r="P16" s="4">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12">
+        <v>3</v>
+      </c>
+      <c r="B17" s="4">
+        <v>9</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3</v>
+      </c>
+      <c r="F17" s="4">
+        <v>4</v>
+      </c>
+      <c r="G17" s="4">
+        <v>5</v>
+      </c>
+      <c r="H17" s="4">
+        <v>6</v>
+      </c>
+      <c r="I17" s="4">
+        <v>7</v>
+      </c>
+      <c r="J17" s="4">
+        <v>8</v>
+      </c>
+      <c r="K17" s="4">
+        <v>9</v>
+      </c>
+      <c r="L17" s="5">
+        <v>1</v>
+      </c>
+      <c r="M17" s="5">
+        <v>2</v>
+      </c>
+      <c r="N17" s="5">
+        <v>3</v>
+      </c>
+      <c r="O17" s="5">
+        <v>4</v>
+      </c>
+      <c r="P17" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12">
+        <v>4</v>
+      </c>
+      <c r="B18" s="5">
+        <v>7</v>
+      </c>
+      <c r="C18" s="5">
+        <v>8</v>
+      </c>
+      <c r="D18" s="5">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <v>2</v>
+      </c>
+      <c r="G18" s="5">
+        <v>3</v>
+      </c>
+      <c r="H18" s="5">
+        <v>4</v>
+      </c>
+      <c r="I18" s="5">
+        <v>5</v>
+      </c>
+      <c r="J18" s="5">
+        <v>6</v>
+      </c>
+      <c r="K18" s="5">
+        <v>7</v>
+      </c>
+      <c r="L18" s="5">
+        <v>8</v>
+      </c>
+      <c r="M18" s="5">
+        <v>9</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12">
+        <v>5</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N20" s="7"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+    </row>
+    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="12">
+        <v>7</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="12"/>
+    </row>
+    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="12">
+        <v>8</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+    </row>
+    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="12">
+        <v>9</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+    </row>
+    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+    </row>
+    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+    </row>
+    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+    </row>
+    <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+    </row>
+    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+    </row>
+    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>